<commit_message>
Added Support for Vertical Certificate & Added GUI
some major changes to code, made orientation selection dynamic
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Rashid </t>
   </si>
   <si>
-    <t xml:space="preserve">02EYEQI1232425</t>
+    <t xml:space="preserve">EYEQ123/24/25</t>
   </si>
 </sst>
 </file>
@@ -115,17 +115,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -320,7 +324,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -347,24 +351,24 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Func to organize files and some fixes
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -32,6 +32,36 @@
   </si>
   <si>
     <t xml:space="preserve">EYEQ123/24/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shahil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EYEQ123/24/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsnush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EYEQ123/24/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iqbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EYEQ123/24/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nikth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EYEQ123/24/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">niktha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EYEQ123/24/30</t>
   </si>
 </sst>
 </file>
@@ -128,7 +158,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,7 +354,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -351,24 +381,44 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>